<commit_message>
Arrancamos con la logica
Prueba de interrupciones externas, programacion del menu principal.
</commit_message>
<xml_diff>
--- a/Mensajes.xlsx
+++ b/Mensajes.xlsx
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P51" sqref="P51"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="U47" sqref="U47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>